<commit_message>
Início da análise exploratória dos dados:
* Análise univariada das variáveis targets;
* Visualização da distribuição dos dados;
* Análise da quantidade de nulos e outliers.
</commit_message>
<xml_diff>
--- a/Questionário de Pesquisa_ Impacto das Redes Sociais na Saúde Mental.xlsx
+++ b/Questionário de Pesquisa_ Impacto das Redes Sociais na Saúde Mental.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27605"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinzen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF132554-E89F-4015-B212-70187CB1143F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{47FA7B9F-36CD-4498-BD57-DA64252E2A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="173">
   <si>
     <t>Id</t>
   </si>
@@ -531,6 +531,30 @@
   </si>
   <si>
     <t xml:space="preserve">Nenhuma dificuldade </t>
+  </si>
+  <si>
+    <t>Contas pessoais de amigos e familiares;Contas de humor e memes;Contas de hobbies e interesses específicos (música, culinária, viagens, etc.)</t>
+  </si>
+  <si>
+    <t>Voluntário</t>
+  </si>
+  <si>
+    <t>Contas pessoais de amigos e familiares;Contas de notícias e política</t>
+  </si>
+  <si>
+    <t>Contas pessoais de amigos e familiares;Contas de humor e memes;Pesquisas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tédio </t>
+  </si>
+  <si>
+    <t>Graduação;Empregado com carteira assinada;Dedicação exclusiva à família</t>
+  </si>
+  <si>
+    <t>Contas pessoais de amigos e familiares;Contas de marcas e empresas;Contas de hobbies e interesses específicos (música, culinária, viagens, etc.)</t>
+  </si>
+  <si>
+    <t>Empregado com carteira assinada;Graduação</t>
   </si>
 </sst>
 </file>
@@ -569,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -578,9 +602,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -732,8 +753,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:AE36" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
-  <autoFilter ref="A1:AE36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:AE42" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A1:AE42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="31">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="30">
       <extLst>
@@ -956,7 +977,7 @@
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{839C7E11-91E4-4DBD-9C5D-0DEA604FA9AC}">
-      <xlmsforms:msForm id="ozd7w-Lp-UK8Z0ubc44d8FBoaAD_OZFDgdXG-ub4lKhURDY1UUlaVFhIUUpRTE05OUIwSVFDTTU1SC4u" isFormConnected="1" maxResponseId="36" latestEventMarker="38">
+      <xlmsforms:msForm id="ozd7w-Lp-UK8Z0ubc44d8FBoaAD_OZFDgdXG-ub4lKhURDY1UUlaVFhIUUpRTE05OUIwSVFDTTU1SC4u" isFormConnected="1" maxResponseId="42" latestEventMarker="46">
         <xlmsforms:syncedQuestionId>id</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>startDate</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>submitDate</xlmsforms:syncedQuestionId>
@@ -1291,10 +1312,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE36"/>
+  <dimension ref="A1:AE42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="W30" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1405,7 +1426,7 @@
       <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
@@ -4389,7 +4410,7 @@
       </c>
     </row>
     <row r="35" spans="1:31" ht="60.75">
-      <c r="A35" s="4">
+      <c r="A35" s="1">
         <v>35</v>
       </c>
       <c r="B35" s="2">
@@ -4405,7 +4426,7 @@
       <c r="F35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="1">
         <v>32</v>
       </c>
       <c r="H35" s="3" t="s">
@@ -4432,10 +4453,10 @@
       <c r="O35" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="P35" s="4">
+      <c r="P35" s="1">
         <v>1</v>
       </c>
-      <c r="Q35" s="4">
+      <c r="Q35" s="1">
         <v>4</v>
       </c>
       <c r="R35" s="3" t="s">
@@ -4444,7 +4465,7 @@
       <c r="S35" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="T35" s="4">
+      <c r="T35" s="1">
         <v>3</v>
       </c>
       <c r="U35" s="3" t="s">
@@ -4456,13 +4477,13 @@
       <c r="W35" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="X35" s="4">
+      <c r="X35" s="1">
         <v>4</v>
       </c>
       <c r="Y35" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="Z35" s="4">
+      <c r="Z35" s="1">
         <v>3</v>
       </c>
       <c r="AA35" s="3" t="s">
@@ -4482,7 +4503,7 @@
       </c>
     </row>
     <row r="36" spans="1:31" ht="45.75">
-      <c r="A36" s="4">
+      <c r="A36" s="1">
         <v>36</v>
       </c>
       <c r="B36" s="2">
@@ -4498,7 +4519,7 @@
       <c r="F36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="1">
         <v>19</v>
       </c>
       <c r="H36" s="3" t="s">
@@ -4525,10 +4546,10 @@
       <c r="O36" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="P36" s="4">
+      <c r="P36" s="1">
         <v>4</v>
       </c>
-      <c r="Q36" s="4">
+      <c r="Q36" s="1">
         <v>2</v>
       </c>
       <c r="R36" s="3" t="s">
@@ -4537,7 +4558,7 @@
       <c r="S36" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="T36" s="4">
+      <c r="T36" s="1">
         <v>1</v>
       </c>
       <c r="U36" s="3" t="s">
@@ -4549,13 +4570,13 @@
       <c r="W36" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="X36" s="4">
+      <c r="X36" s="1">
         <v>2</v>
       </c>
       <c r="Y36" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="Z36" s="4">
+      <c r="Z36" s="1">
         <v>2</v>
       </c>
       <c r="AA36" s="3" t="s">
@@ -4573,6 +4594,498 @@
       <c r="AE36" s="3" t="s">
         <v>164</v>
       </c>
+    </row>
+    <row r="37" spans="1:31" ht="30.75">
+      <c r="A37" s="1">
+        <v>37</v>
+      </c>
+      <c r="B37" s="2">
+        <v>45386.855104166701</v>
+      </c>
+      <c r="C37" s="2">
+        <v>45386.855543981503</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" s="1">
+        <v>19</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="3"/>
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="3"/>
+      <c r="AB37" s="3"/>
+      <c r="AC37" s="3"/>
+      <c r="AD37" s="3"/>
+      <c r="AE37" s="3"/>
+    </row>
+    <row r="38" spans="1:31" ht="45.75">
+      <c r="A38" s="1">
+        <v>38</v>
+      </c>
+      <c r="B38" s="2">
+        <v>45386.966041666703</v>
+      </c>
+      <c r="C38" s="2">
+        <v>45386.969189814801</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38" s="1">
+        <v>50</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O38" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P38" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>1</v>
+      </c>
+      <c r="R38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="T38" s="1">
+        <v>1</v>
+      </c>
+      <c r="U38" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="X38" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z38" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA38" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB38" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC38" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD38" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE38" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" ht="30.75">
+      <c r="A39" s="1">
+        <v>39</v>
+      </c>
+      <c r="B39" s="2">
+        <v>45386.972500000003</v>
+      </c>
+      <c r="C39" s="2">
+        <v>45386.979270833297</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G39" s="1">
+        <v>43</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P39" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>1</v>
+      </c>
+      <c r="R39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S39" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="T39" s="1">
+        <v>1</v>
+      </c>
+      <c r="U39" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V39" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="W39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X39" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y39" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z39" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB39" s="3"/>
+      <c r="AC39" s="3"/>
+      <c r="AD39" s="3"/>
+      <c r="AE39" s="3"/>
+    </row>
+    <row r="40" spans="1:31" ht="30.75">
+      <c r="A40" s="1">
+        <v>40</v>
+      </c>
+      <c r="B40" s="2">
+        <v>45387.427581018499</v>
+      </c>
+      <c r="C40" s="2">
+        <v>45387.4291898148</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G40" s="1">
+        <v>19</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O40" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P40" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>5</v>
+      </c>
+      <c r="R40" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S40" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="T40" s="1">
+        <v>2</v>
+      </c>
+      <c r="U40" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="V40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W40" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X40" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y40" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z40" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA40" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC40" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD40" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE40" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" ht="45.75">
+      <c r="A41" s="1">
+        <v>41</v>
+      </c>
+      <c r="B41" s="2">
+        <v>45387.563252314802</v>
+      </c>
+      <c r="C41" s="2">
+        <v>45387.567395833299</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" s="1">
+        <v>18</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P41" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>5</v>
+      </c>
+      <c r="R41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S41" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="T41" s="1">
+        <v>1</v>
+      </c>
+      <c r="U41" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W41" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X41" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z41" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB41" s="3"/>
+      <c r="AC41" s="3"/>
+      <c r="AD41" s="3"/>
+      <c r="AE41" s="3"/>
+    </row>
+    <row r="42" spans="1:31" ht="30.75">
+      <c r="A42" s="1">
+        <v>42</v>
+      </c>
+      <c r="B42" s="2">
+        <v>45387.654560185198</v>
+      </c>
+      <c r="C42" s="2">
+        <v>45387.656041666698</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G42" s="1">
+        <v>19</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O42" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P42" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>1</v>
+      </c>
+      <c r="R42" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S42" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="T42" s="1">
+        <v>4</v>
+      </c>
+      <c r="U42" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="V42" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="W42" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X42" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y42" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z42" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB42" s="3"/>
+      <c r="AC42" s="3"/>
+      <c r="AD42" s="3"/>
+      <c r="AE42" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Limpeza e Tratamento de Outliers
</commit_message>
<xml_diff>
--- a/Questionário de Pesquisa_ Impacto das Redes Sociais na Saúde Mental.xlsx
+++ b/Questionário de Pesquisa_ Impacto das Redes Sociais na Saúde Mental.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27605"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27618"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinzen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47FA7B9F-36CD-4498-BD57-DA64252E2A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C0ECBB3-3567-45B7-8EF2-BD695CCEEA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="200">
   <si>
     <t>Id</t>
   </si>
@@ -555,6 +555,88 @@
   </si>
   <si>
     <t>Empregado com carteira assinada;Graduação</t>
+  </si>
+  <si>
+    <t>Contas pessoais de amigos e familiares;Contas de notícias e política;Contas de hobbies e interesses específicos (música, culinária, viagens, etc.)</t>
+  </si>
+  <si>
+    <t>Desinstalar aplicativos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eu não tenho tanta dificuldade em reduzir o tempo no celular, as vzs ate esqueço. </t>
+  </si>
+  <si>
+    <t>Graduação;Bolsista;Voluntário;Empregado com carteira assinada</t>
+  </si>
+  <si>
+    <t>Instagram;WhatsApp;Twitter</t>
+  </si>
+  <si>
+    <t>Contas pessoais de amigos e familiares;Contas de celebridades e influenciadores;Contas de marcas e empresas;Contas de humor e memes;Contas de notícias e política;Contas de esportes;Contas de hobbies e interesses específicos (música, culinária, viagens, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">esquecer da existencia do celular e esque eu poderia estar recebendo uma mensagem muito importante de algum familiar ou da faculdade. Na verdade dentro de um determinado tempo eu fico uma semana sem tocar no meu celular. 
+</t>
+  </si>
+  <si>
+    <t>Desativar notificações;Limitar o tempo de uso</t>
+  </si>
+  <si>
+    <t>Depender do celular para me comunicar com amigos, colegas de trabalho e de estudo.</t>
+  </si>
+  <si>
+    <t>Graduação;Professor PSS</t>
+  </si>
+  <si>
+    <t>Contas pessoais de amigos e familiares;Contas de humor e memes;Contas de notícias e política;Contas de esportes</t>
+  </si>
+  <si>
+    <t>Desativar notificações;Limitar o tempo de uso;Buscar ajuda profissional</t>
+  </si>
+  <si>
+    <t>WhatsApp;Instagram;YouTube</t>
+  </si>
+  <si>
+    <t>Contas pessoais de amigos e familiares;Contas de humor e memes;Contas de esportes;Contas de hobbies e interesses específicos (música, culinária, viagens, etc.)</t>
+  </si>
+  <si>
+    <t>estar desconectado do mundo</t>
+  </si>
+  <si>
+    <t>Contas pessoais de amigos e familiares;Contas de humor e memes;Contas de esportes;Contas de marcas e empresas</t>
+  </si>
+  <si>
+    <t>Instagram;Facebook;WhatsApp;YouTube;TikTok</t>
+  </si>
+  <si>
+    <t>Desinstalar aplicativos;Limitar o tempo de uso</t>
+  </si>
+  <si>
+    <t>Não, eu não consinto em utilizar minhas respostas para fins de pesquisa.</t>
+  </si>
+  <si>
+    <t>Graduação;Estagiário</t>
+  </si>
+  <si>
+    <t>Contas pessoais de amigos e familiares;Contas de marcas e empresas;Contas de esportes</t>
+  </si>
+  <si>
+    <t>Graduação;Empregado com carteira assinada;Bolsista;Voluntário</t>
+  </si>
+  <si>
+    <t>Contas de humor e memes;Contas de notícias e política;Contas de hobbies e interesses específicos (música, culinária, viagens, etc.);Contas pessoais de amigos e familiares</t>
+  </si>
+  <si>
+    <t>Simplesmente tédio</t>
+  </si>
+  <si>
+    <t>WhatsApp;Instagram;Facebook;YouTube</t>
+  </si>
+  <si>
+    <t>cumprir tempo limitado do uso.</t>
+  </si>
+  <si>
+    <t>Tédio e necessidade de usar o mesmo para fins de faculdade</t>
   </si>
 </sst>
 </file>
@@ -593,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -602,6 +684,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -753,8 +838,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:AE42" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
-  <autoFilter ref="A1:AE42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:AE58" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A1:AE58" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="31">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="30">
       <extLst>
@@ -977,7 +1062,7 @@
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext xmlns:xlmsforms="http://schemas.microsoft.com/office/spreadsheetml/2023/msForms" uri="{839C7E11-91E4-4DBD-9C5D-0DEA604FA9AC}">
-      <xlmsforms:msForm id="ozd7w-Lp-UK8Z0ubc44d8FBoaAD_OZFDgdXG-ub4lKhURDY1UUlaVFhIUUpRTE05OUIwSVFDTTU1SC4u" isFormConnected="1" maxResponseId="42" latestEventMarker="46">
+      <xlmsforms:msForm id="ozd7w-Lp-UK8Z0ubc44d8FBoaAD_OZFDgdXG-ub4lKhURDY1UUlaVFhIUUpRTE05OUIwSVFDTTU1SC4u" isFormConnected="1" maxResponseId="58" latestEventMarker="62">
         <xlmsforms:syncedQuestionId>id</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>startDate</xlmsforms:syncedQuestionId>
         <xlmsforms:syncedQuestionId>submitDate</xlmsforms:syncedQuestionId>
@@ -1312,9 +1397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE42"/>
+  <dimension ref="A1:AE58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W30" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
       <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
@@ -5087,6 +5172,1398 @@
       <c r="AD42" s="3"/>
       <c r="AE42" s="3"/>
     </row>
+    <row r="43" spans="1:31" ht="45.75">
+      <c r="A43" s="1">
+        <v>43</v>
+      </c>
+      <c r="B43" s="2">
+        <v>45388.555393518502</v>
+      </c>
+      <c r="C43" s="2">
+        <v>45388.559212963002</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" s="1">
+        <v>21</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O43" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P43" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>5</v>
+      </c>
+      <c r="R43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S43" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="T43" s="1">
+        <v>4</v>
+      </c>
+      <c r="U43" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="V43" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="W43" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X43" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y43" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z43" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB43" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC43" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE43" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" ht="30.75">
+      <c r="A44" s="1">
+        <v>44</v>
+      </c>
+      <c r="B44" s="2">
+        <v>45389.503773148099</v>
+      </c>
+      <c r="C44" s="2">
+        <v>45389.506782407399</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G44" s="1">
+        <v>19</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O44" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P44" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>3</v>
+      </c>
+      <c r="R44" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S44" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="T44" s="1">
+        <v>2</v>
+      </c>
+      <c r="U44" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="V44" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W44" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X44" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y44" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z44" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA44" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB44" s="3"/>
+      <c r="AC44" s="3"/>
+      <c r="AD44" s="3"/>
+      <c r="AE44" s="3"/>
+    </row>
+    <row r="45" spans="1:31" ht="91.5">
+      <c r="A45" s="1">
+        <v>45</v>
+      </c>
+      <c r="B45" s="2">
+        <v>45389.686909722201</v>
+      </c>
+      <c r="C45" s="2">
+        <v>45389.692199074103</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G45" s="1">
+        <v>25</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O45" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P45" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>2</v>
+      </c>
+      <c r="R45" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S45" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="T45" s="1">
+        <v>1</v>
+      </c>
+      <c r="U45" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="V45" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W45" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="X45" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y45" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z45" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA45" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC45" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD45" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE45" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" ht="91.5">
+      <c r="A46" s="1">
+        <v>46</v>
+      </c>
+      <c r="B46" s="2">
+        <v>45389.828055555598</v>
+      </c>
+      <c r="C46" s="2">
+        <v>45389.829826388901</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" s="1">
+        <v>21</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O46" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P46" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>4</v>
+      </c>
+      <c r="R46" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S46" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="T46" s="1">
+        <v>3</v>
+      </c>
+      <c r="U46" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V46" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W46" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X46" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y46" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z46" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA46" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB46" s="3"/>
+      <c r="AC46" s="3"/>
+      <c r="AD46" s="3"/>
+      <c r="AE46" s="3"/>
+    </row>
+    <row r="47" spans="1:31" ht="45.75">
+      <c r="A47" s="1">
+        <v>47</v>
+      </c>
+      <c r="B47" s="2">
+        <v>45389.972210648099</v>
+      </c>
+      <c r="C47" s="2">
+        <v>45389.977407407401</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G47" s="1">
+        <v>24</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O47" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P47" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>4</v>
+      </c>
+      <c r="R47" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S47" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T47" s="1">
+        <v>2</v>
+      </c>
+      <c r="U47" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="V47" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W47" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X47" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y47" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z47" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA47" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB47" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC47" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="AD47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE47" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" ht="45.75">
+      <c r="A48" s="1">
+        <v>48</v>
+      </c>
+      <c r="B48" s="2">
+        <v>45390.4542013889</v>
+      </c>
+      <c r="C48" s="2">
+        <v>45390.456122685202</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G48" s="1">
+        <v>31</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O48" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P48" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>5</v>
+      </c>
+      <c r="R48" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="T48" s="1">
+        <v>5</v>
+      </c>
+      <c r="U48" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="V48" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="W48" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X48" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y48" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z48" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA48" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB48" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC48" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="AD48" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE48" s="3"/>
+    </row>
+    <row r="49" spans="1:31" ht="60.75">
+      <c r="A49" s="1">
+        <v>49</v>
+      </c>
+      <c r="B49" s="2">
+        <v>45390.678460648203</v>
+      </c>
+      <c r="C49" s="2">
+        <v>45390.682592592602</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G49" s="1">
+        <v>23</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P49" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>2</v>
+      </c>
+      <c r="R49" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S49" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="T49" s="1">
+        <v>1</v>
+      </c>
+      <c r="U49" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="V49" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="W49" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="X49" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y49" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z49" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA49" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC49" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE49" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" ht="45.75">
+      <c r="A50" s="1">
+        <v>50</v>
+      </c>
+      <c r="B50" s="2">
+        <v>45390.8181944444</v>
+      </c>
+      <c r="C50" s="2">
+        <v>45390.822766203702</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G50" s="1">
+        <v>23</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M50" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N50" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O50" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P50" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>5</v>
+      </c>
+      <c r="R50" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S50" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="T50" s="1">
+        <v>2</v>
+      </c>
+      <c r="U50" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V50" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W50" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X50" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y50" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z50" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA50" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB50" s="3"/>
+      <c r="AC50" s="3"/>
+      <c r="AD50" s="3"/>
+      <c r="AE50" s="3"/>
+    </row>
+    <row r="51" spans="1:31" ht="60.75">
+      <c r="A51" s="4">
+        <v>51</v>
+      </c>
+      <c r="B51" s="2">
+        <v>45391.625023148197</v>
+      </c>
+      <c r="C51" s="2">
+        <v>45391.627754629597</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G51" s="4">
+        <v>18</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M51" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N51" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O51" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P51" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>2</v>
+      </c>
+      <c r="R51" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S51" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="T51" s="4">
+        <v>1</v>
+      </c>
+      <c r="U51" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V51" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="W51" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X51" s="4">
+        <v>3</v>
+      </c>
+      <c r="Y51" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z51" s="4">
+        <v>2</v>
+      </c>
+      <c r="AA51" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC51" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE51" s="3"/>
+    </row>
+    <row r="52" spans="1:31" ht="91.5">
+      <c r="A52" s="4">
+        <v>52</v>
+      </c>
+      <c r="B52" s="2">
+        <v>45391.790509259299</v>
+      </c>
+      <c r="C52" s="2">
+        <v>45391.791388888902</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G52" s="4">
+        <v>21</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M52" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N52" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P52" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q52" s="4">
+        <v>3</v>
+      </c>
+      <c r="R52" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S52" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="T52" s="4">
+        <v>3</v>
+      </c>
+      <c r="U52" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V52" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W52" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X52" s="4">
+        <v>3</v>
+      </c>
+      <c r="Y52" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z52" s="4">
+        <v>3</v>
+      </c>
+      <c r="AA52" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB52" s="3"/>
+      <c r="AC52" s="3"/>
+      <c r="AD52" s="3"/>
+      <c r="AE52" s="3"/>
+    </row>
+    <row r="53" spans="1:31" ht="30.75">
+      <c r="A53" s="4">
+        <v>53</v>
+      </c>
+      <c r="B53" s="2">
+        <v>45392.835335648197</v>
+      </c>
+      <c r="C53" s="2">
+        <v>45392.835810185199</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="G53" s="4"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" s="4"/>
+      <c r="U53" s="3"/>
+      <c r="V53" s="3"/>
+      <c r="W53" s="3"/>
+      <c r="X53" s="4"/>
+      <c r="Y53" s="3"/>
+      <c r="Z53" s="4"/>
+      <c r="AA53" s="3"/>
+      <c r="AB53" s="3"/>
+      <c r="AC53" s="3"/>
+      <c r="AD53" s="3"/>
+      <c r="AE53" s="3"/>
+    </row>
+    <row r="54" spans="1:31" ht="30.75">
+      <c r="A54" s="4">
+        <v>54</v>
+      </c>
+      <c r="B54" s="2">
+        <v>45394.873807870397</v>
+      </c>
+      <c r="C54" s="2">
+        <v>45394.877210648097</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" s="4">
+        <v>20</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M54" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N54" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O54" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P54" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q54" s="4">
+        <v>5</v>
+      </c>
+      <c r="R54" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S54" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="T54" s="4">
+        <v>4</v>
+      </c>
+      <c r="U54" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="V54" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W54" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X54" s="4">
+        <v>4</v>
+      </c>
+      <c r="Y54" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z54" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA54" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB54" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC54" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AD54" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE54" s="3"/>
+    </row>
+    <row r="55" spans="1:31" ht="30.75">
+      <c r="A55" s="4">
+        <v>55</v>
+      </c>
+      <c r="B55" s="2">
+        <v>45396.809664351902</v>
+      </c>
+      <c r="C55" s="2">
+        <v>45396.811909722201</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G55" s="4">
+        <v>24</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="L55" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M55" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O55" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P55" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q55" s="4">
+        <v>3</v>
+      </c>
+      <c r="R55" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S55" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="T55" s="4">
+        <v>2</v>
+      </c>
+      <c r="U55" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V55" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W55" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="X55" s="4">
+        <v>2</v>
+      </c>
+      <c r="Y55" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z55" s="4">
+        <v>2</v>
+      </c>
+      <c r="AA55" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB55" s="3"/>
+      <c r="AC55" s="3"/>
+      <c r="AD55" s="3"/>
+      <c r="AE55" s="3"/>
+    </row>
+    <row r="56" spans="1:31" ht="60.75">
+      <c r="A56" s="4">
+        <v>56</v>
+      </c>
+      <c r="B56" s="2">
+        <v>45397.635185185201</v>
+      </c>
+      <c r="C56" s="2">
+        <v>45397.638124999998</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G56" s="4">
+        <v>23</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M56" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O56" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P56" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q56" s="4">
+        <v>4</v>
+      </c>
+      <c r="R56" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S56" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="T56" s="4">
+        <v>4</v>
+      </c>
+      <c r="U56" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="V56" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="W56" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X56" s="4">
+        <v>4</v>
+      </c>
+      <c r="Y56" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z56" s="4">
+        <v>3</v>
+      </c>
+      <c r="AA56" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB56" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC56" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD56" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE56" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" ht="91.5">
+      <c r="A57" s="4">
+        <v>57</v>
+      </c>
+      <c r="B57" s="2">
+        <v>45397.952893518501</v>
+      </c>
+      <c r="C57" s="2">
+        <v>45397.956458333298</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G57" s="4">
+        <v>23</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M57" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N57" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O57" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P57" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q57" s="4">
+        <v>1</v>
+      </c>
+      <c r="R57" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S57" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="T57" s="4">
+        <v>1</v>
+      </c>
+      <c r="U57" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="V57" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W57" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="X57" s="4">
+        <v>2</v>
+      </c>
+      <c r="Y57" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z57" s="4">
+        <v>3</v>
+      </c>
+      <c r="AA57" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB57" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC57" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD57" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE57" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31" ht="30.75">
+      <c r="A58" s="4">
+        <v>58</v>
+      </c>
+      <c r="B58" s="2">
+        <v>45400.360983796301</v>
+      </c>
+      <c r="C58" s="2">
+        <v>45400.365231481497</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G58" s="4">
+        <v>24</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M58" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N58" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P58" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q58" s="4">
+        <v>3</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S58" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="T58" s="4">
+        <v>1</v>
+      </c>
+      <c r="U58" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V58" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W58" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X58" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y58" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z58" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA58" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB58" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC58" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD58" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE58" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>